<commit_message>
update BOM only 1k resistor is needed
</commit_message>
<xml_diff>
--- a/Neon_2x1M_12V/components_checklist_Neon_2x1M_12V.xlsx
+++ b/Neon_2x1M_12V/components_checklist_Neon_2x1M_12V.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\NEON_2x1M\Neon_2x1M_12V\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E494370C-1117-44E4-9F84-E7A65A89F23E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68AD88F-2DD5-4793-8200-F02F04F69A7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="41280" windowHeight="13260"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="41280" windowHeight="13260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="components_checklist_Neon_2x1M_" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="90">
   <si>
     <t>Reference</t>
   </si>
@@ -181,12 +181,6 @@
     <t>Q3</t>
   </si>
   <si>
-    <t>BSS138</t>
-  </si>
-  <si>
-    <t>https://makerselectronics.com/product/smd-mosfet-transistor-bss138-j1-50v-220ma-3-5%CF%8910v220ma-360mw-n-channel-sot-23/?srsltid=AfmBOorKPkIxsAwv-3Onwyym6kfiJ7AE8Pv9g0Pld8GAUTAgILHxbmr_</t>
-  </si>
-  <si>
     <t>Q4,Q5</t>
   </si>
   <si>
@@ -196,15 +190,9 @@
     <t>R1</t>
   </si>
   <si>
-    <t>2.2k Ohm</t>
-  </si>
-  <si>
     <t>Resistor_SMD:R_1206_3216Metric_Pad1.30x1.75mm_HandSolder</t>
   </si>
   <si>
-    <t>https://makerselectronics.com/product/chip-resistor-smd-2-2k%cf%89-%c2%b15-250mw-1206/</t>
-  </si>
-  <si>
     <t>R2,R5</t>
   </si>
   <si>
@@ -232,9 +220,6 @@
     <t>1k Ohm</t>
   </si>
   <si>
-    <t>https://makerselectronics.com/product/chip-resistor-smd-1k%cf%89-%c2%b15-0-25w-%c2%b1100ppm-%e2%84%83-1206-chip/</t>
-  </si>
-  <si>
     <t>R9,R14,R15,R19</t>
   </si>
   <si>
@@ -250,18 +235,9 @@
     <t>220 Ohm</t>
   </si>
   <si>
-    <t>https://uge-one.com/product/smd-chip-resistor-size-1206-220r-ohm/?srsltid=AfmBOoqmkuXwKrfJ3VxJ5AIPn5xc8j2ZOYO0PqRCmSUCAxMBlBADOpRb</t>
-  </si>
-  <si>
     <t>R13</t>
   </si>
   <si>
-    <t>660 Ohm</t>
-  </si>
-  <si>
-    <t>https://makerselectronics.com/product/chip-resistor-smd-680%cf%89-%c2%b11-250mw-1206/</t>
-  </si>
-  <si>
     <t>SW1,SW2</t>
   </si>
   <si>
@@ -296,13 +272,31 @@
   </si>
   <si>
     <t>https://uge-one.com/product/xl1509-3-3e1-2a-150khz-buck-dc-dc-step-down-converter-regulator-ic-smd/?srsltid=AfmBOoo-d0v4w8P7LjpvPGnwJM-lnyFaeHPU-1Q8rCWLEaeI_F_a5hk3</t>
+  </si>
+  <si>
+    <t>680 Ohm</t>
+  </si>
+  <si>
+    <t>https://uge-one.com/product/smd-chip-resistor-size-1206-680r-ohm/</t>
+  </si>
+  <si>
+    <t>https://uge-one.com/product/smd-chip-resistor-size-1206-220r-ohm/</t>
+  </si>
+  <si>
+    <t>https://uge-one.com/product/smd-chip-resistor-size-1206-1k-ohm-1/</t>
+  </si>
+  <si>
+    <t>https://uge-one.com/product/si2302ds-sot23-general-purpose-n-channel-mosfet-smd-transistor-sot-23/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si2302DS </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -433,6 +427,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -735,7 +737,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -778,13 +780,15 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -818,6 +822,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1137,11 +1142,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1213,7 +1218,7 @@
         <v>16</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" t="s">
+      <c r="I3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1387,7 +1392,9 @@
       <c r="G12" t="s">
         <v>50</v>
       </c>
-      <c r="H12" s="2"/>
+      <c r="H12" s="2">
+        <v>7</v>
+      </c>
       <c r="I12" t="s">
         <v>51</v>
       </c>
@@ -1400,223 +1407,250 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="G13" t="s">
         <v>50</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" t="s">
-        <v>54</v>
+      <c r="H13" s="2">
+        <v>8</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="G14" t="s">
-        <v>56</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="I14" t="s">
         <v>54</v>
+      </c>
+      <c r="H14" s="2">
+        <v>9</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="G15" t="s">
-        <v>59</v>
-      </c>
-      <c r="H15" s="2"/>
-      <c r="I15" t="s">
-        <v>60</v>
+        <v>56</v>
+      </c>
+      <c r="H15" s="2">
+        <v>6</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G16" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="2">
+        <v>5</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="H16" s="2"/>
-      <c r="I16" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B17">
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G17" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I17" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G18" t="s">
-        <v>59</v>
-      </c>
-      <c r="H18" s="2"/>
-      <c r="I18" t="s">
-        <v>70</v>
+        <v>56</v>
+      </c>
+      <c r="H18" s="2">
+        <v>4</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G19" t="s">
-        <v>59</v>
-      </c>
-      <c r="H19" s="2"/>
-      <c r="I19" t="s">
-        <v>73</v>
+        <v>56</v>
+      </c>
+      <c r="H19" s="2">
+        <v>3</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B20">
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G20" t="s">
-        <v>59</v>
-      </c>
-      <c r="H20" s="2"/>
-      <c r="I20" t="s">
-        <v>76</v>
+        <v>56</v>
+      </c>
+      <c r="H20" s="2">
+        <v>2</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="G21" t="s">
-        <v>59</v>
-      </c>
-      <c r="H21" s="2"/>
-      <c r="I21" t="s">
-        <v>79</v>
+        <v>56</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G22" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I22" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G23" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I23" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="G24" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I24" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I3" r:id="rId1" xr:uid="{DEEAB395-A983-4B81-B43B-897DD4B22539}"/>
+    <hyperlink ref="I21" r:id="rId2" xr:uid="{FE68C376-9274-4248-89C4-B00DC415872B}"/>
+    <hyperlink ref="I20" r:id="rId3" xr:uid="{8E99F32B-34B5-4567-9791-E8177D0A90CA}"/>
+    <hyperlink ref="I19" r:id="rId4" xr:uid="{02A3B365-95D9-4FB2-8C7D-AFE698C0B5D6}"/>
+    <hyperlink ref="I18" r:id="rId5" xr:uid="{A01FA37C-C9D8-4195-83C2-A3ED298FBAC4}"/>
+    <hyperlink ref="I16" r:id="rId6" xr:uid="{0EF25ED2-7119-4766-89BF-13FE2667934F}"/>
+    <hyperlink ref="I15" r:id="rId7" xr:uid="{24E25FC7-4895-4ACA-9393-C91C51F54509}"/>
+    <hyperlink ref="I13" r:id="rId8" xr:uid="{2354A54C-0CBB-4446-9EEA-90D681A801B6}"/>
+    <hyperlink ref="I14" r:id="rId9" xr:uid="{F0A07871-F761-4036-A985-1B494AF1AA0D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed blue led and replaced it with red one and also updated their current imiting resistor
</commit_message>
<xml_diff>
--- a/Neon_2x1M_12V/components_checklist_Neon_2x1M_12V.xlsx
+++ b/Neon_2x1M_12V/components_checklist_Neon_2x1M_12V.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\NEON_2x1M\Neon_2x1M_12V\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68AD88F-2DD5-4793-8200-F02F04F69A7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643EFC9C-53DA-44D0-88A6-AF9D1EE04593}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="41280" windowHeight="13260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,9 +73,6 @@
     <t>Capacitor_THT:CP_Radial_D10.0mm_P5.00mm</t>
   </si>
   <si>
-    <t>https://makerselectronics.com/product/capacitor-470uf-35v-1016mm/?srsltid=AfmBOor09AGOe6uRfUPUSJ8gQ4mHe95vw-zHcd40OwpcpkuWNsINe4Bm</t>
-  </si>
-  <si>
     <t>C3</t>
   </si>
   <si>
@@ -217,9 +214,6 @@
     <t>R4</t>
   </si>
   <si>
-    <t>1k Ohm</t>
-  </si>
-  <si>
     <t>R9,R14,R15,R19</t>
   </si>
   <si>
@@ -283,13 +277,19 @@
     <t>https://uge-one.com/product/smd-chip-resistor-size-1206-220r-ohm/</t>
   </si>
   <si>
-    <t>https://uge-one.com/product/smd-chip-resistor-size-1206-1k-ohm-1/</t>
-  </si>
-  <si>
     <t>https://uge-one.com/product/si2302ds-sot23-general-purpose-n-channel-mosfet-smd-transistor-sot-23/</t>
   </si>
   <si>
     <t xml:space="preserve">Si2302DS </t>
+  </si>
+  <si>
+    <t>https://uge-one.com/product/smd-chip-resistor-size-1206-820r-ohm/</t>
+  </si>
+  <si>
+    <t>820 Ohm</t>
+  </si>
+  <si>
+    <t>https://www.ram-e-shop.com/ar/shop/c-470u50v-capacitor-mkthf-kymyyy-470uf-mykrw-frd-50v-fwlt-6096?srsltid=AfmBOoqRsYbzCBVtm-slOtdkZkF3_VHsxGuC_knYwLzqNao195TnxDGK</t>
   </si>
 </sst>
 </file>
@@ -1146,7 +1146,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1219,121 +1219,121 @@
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="3" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
         <v>19</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
         <v>23</v>
-      </c>
-      <c r="G5" t="s">
-        <v>24</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
         <v>27</v>
-      </c>
-      <c r="G6" t="s">
-        <v>28</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" t="s">
         <v>34</v>
-      </c>
-      <c r="G8" t="s">
-        <v>35</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
       <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" t="s">
         <v>38</v>
-      </c>
-      <c r="G9" t="s">
-        <v>39</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>12</v>
@@ -1341,116 +1341,116 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" t="s">
         <v>41</v>
-      </c>
-      <c r="G10" t="s">
-        <v>42</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" t="s">
         <v>45</v>
-      </c>
-      <c r="G11" t="s">
-        <v>46</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" t="s">
         <v>49</v>
-      </c>
-      <c r="G12" t="s">
-        <v>50</v>
       </c>
       <c r="H12" s="2">
         <v>7</v>
       </c>
-      <c r="I12" t="s">
-        <v>51</v>
+      <c r="I12" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H13" s="2">
         <v>8</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H14" s="2">
         <v>9</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="G15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H15" s="2">
         <v>6</v>
@@ -1461,56 +1461,56 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H16" s="2">
         <v>5</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17">
         <v>7</v>
       </c>
       <c r="C17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" t="s">
         <v>61</v>
-      </c>
-      <c r="G17" t="s">
-        <v>62</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="G18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H18" s="2">
         <v>4</v>
@@ -1521,122 +1521,122 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H19" s="2">
         <v>3</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B20">
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H20" s="2">
         <v>2</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H21" s="2">
         <v>1</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1650,6 +1650,7 @@
     <hyperlink ref="I15" r:id="rId7" xr:uid="{24E25FC7-4895-4ACA-9393-C91C51F54509}"/>
     <hyperlink ref="I13" r:id="rId8" xr:uid="{2354A54C-0CBB-4446-9EEA-90D681A801B6}"/>
     <hyperlink ref="I14" r:id="rId9" xr:uid="{F0A07871-F761-4036-A985-1B494AF1AA0D}"/>
+    <hyperlink ref="I12" r:id="rId10" xr:uid="{670D436D-9FFC-4A7C-BA3C-6B1088A2F99B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>